<commit_message>
fixed a dumb error in summary stat table
</commit_message>
<xml_diff>
--- a/part2_exploratory_analysis/summary stats.xlsx
+++ b/part2_exploratory_analysis/summary stats.xlsx
@@ -492,8 +492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:V38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="U10" sqref="U10"/>
+    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -632,7 +632,7 @@
         <v>29</v>
       </c>
       <c r="S6">
-        <v>193</v>
+        <v>15794</v>
       </c>
       <c r="T6">
         <v>1</v>
@@ -664,7 +664,7 @@
         <v>30</v>
       </c>
       <c r="S7">
-        <v>15794</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.2">

</xml_diff>